<commit_message>
Updated Sprint 3 Burndown
1) I updated the sprint backlog to reflect our main backlog.
2) This should be up to date with where we currently are.
</commit_message>
<xml_diff>
--- a/sprints/Sprint3/sprint3_backlog.xlsx
+++ b/sprints/Sprint3/sprint3_backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drivera3\source\repos\CapstoneProjectGroup7\sprints\Sprint3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\CapstoneProjectGroup7\sprints\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9E3EBE-235F-4DD7-9F6E-7EEF45676890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EB798C-BF66-49D4-9763-3C6111EA7A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Related User Story</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Amount Remaining After…</t>
   </si>
   <si>
-    <t>edit group/ project should assign member/group using separate box for list of options and list of currently selected items</t>
-  </si>
-  <si>
     <t>Assigned To</t>
   </si>
   <si>
@@ -68,22 +65,34 @@
     <t>View Task</t>
   </si>
   <si>
-    <t>Create Task</t>
-  </si>
-  <si>
-    <t>Update Stage for Task</t>
-  </si>
-  <si>
-    <t>Assign Task</t>
-  </si>
-  <si>
-    <t>&lt;OPTIONAL&gt; display history for task on view (aka log)</t>
-  </si>
-  <si>
-    <t>&lt;OPTIONAL&gt; post comment for task</t>
-  </si>
-  <si>
-    <t>Restrict Column to group</t>
+    <t>Edit Group</t>
+  </si>
+  <si>
+    <t>Edit Project</t>
+  </si>
+  <si>
+    <t>Assign/Remove Group to/from Project</t>
+  </si>
+  <si>
+    <t>Assign a task to myself</t>
+  </si>
+  <si>
+    <t>Create a Task on the Board of a Project for my Group</t>
+  </si>
+  <si>
+    <t>Update Stage of my assigned Task</t>
+  </si>
+  <si>
+    <t>Assign a Task on a Board from a Project for my Group to an Employee in my Group</t>
+  </si>
+  <si>
+    <t>Assign/Remove Group(s) to/from Stage of Project</t>
+  </si>
+  <si>
+    <t>View a history of events for a Task (Optional)</t>
+  </si>
+  <si>
+    <t>Post a comment to a Task on the Board of a Project for my Group (Optional)</t>
   </si>
 </sst>
 </file>
@@ -286,18 +295,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$11:$E$11</c:f>
+              <c:f>Sheet1!$C$14:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1047,7 +1056,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>182562</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1339,21 +1348,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1368,10 +1377,10 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="4" t="s">
@@ -1381,15 +1390,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1398,66 +1407,66 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -1466,43 +1475,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="C10" s="6">
         <v>2</v>
       </c>
@@ -1513,18 +1526,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="3">
-        <f>SUM(C3:C10)</f>
-        <v>15</v>
-      </c>
-      <c r="D11" s="2">
-        <f>SUM(D3:D10)</f>
-        <v>10</v>
-      </c>
-      <c r="E11" s="2">
-        <f>SUM(E3:E10)</f>
-        <v>4</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C14" s="3">
+        <f>SUM(C3:C13)</f>
+        <v>20</v>
+      </c>
+      <c r="D14" s="2">
+        <f>SUM(D3:D13)</f>
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <f>SUM(E3:E13)</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sprint Backlog and fully tested the controllers
</commit_message>
<xml_diff>
--- a/sprints/Sprint3/sprint3_backlog.xlsx
+++ b/sprints/Sprint3/sprint3_backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drivera3\source\repos\CapstoneProjectGroup7\sprints\Sprint3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\CapstoneProjectGroup7\sprints\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E8080B-2924-4135-B2EB-C4ECB98BDE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDC0353-7238-4B47-8FC1-CEB150213BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38610" windowHeight="20295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5350" yWindow="4220" windowWidth="28800" windowHeight="15410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1351,18 +1351,18 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -1390,7 +1390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -1523,15 +1523,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -1543,7 +1543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C14" s="3">
         <f>SUM(C3:C13)</f>
         <v>20</v>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="E14" s="2">
         <f>SUM(E3:E13)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>